<commit_message>
Update classification report with new metrics and revise validation metadata
</commit_message>
<xml_diff>
--- a/video_label_summary_validation_metadata.xlsx
+++ b/video_label_summary_validation_metadata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,17 +468,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>dataset/val\Distraction\3930172_dms_drowsy_4.mp4</t>
+          <t>dataset/val\Drowsy\360326202501_dms_drowsy_12.mp4</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="C2" t="n">
-        <v>77</v>
+        <v>197</v>
       </c>
       <c r="D2" t="n">
-        <v>164</v>
+        <v>32</v>
       </c>
       <c r="E2" t="n">
         <v>2</v>
@@ -490,42 +490,42 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>dataset/val\Distraction\3930172_dms_drowsy_6.mp4</t>
+          <t>dataset/val\Drowsy\3934336_dms_drowsy_1.mp4</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>217</v>
+        <v>306</v>
       </c>
       <c r="C3" t="n">
-        <v>119</v>
+        <v>299</v>
       </c>
       <c r="D3" t="n">
-        <v>98</v>
+        <v>6</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>dataset/val\Distraction\3932842_dms_drowsy_1.mp4</t>
+          <t>dataset/val\Drowsy\3935656_dms_drowsy_1.mp4</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="C4" t="n">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="D4" t="n">
-        <v>133</v>
+        <v>94</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="F4" t="n">
         <v>10</v>
@@ -534,20 +534,20 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>dataset/val\Distraction\3935656_dms_drowsy_4.mp4</t>
+          <t>dataset/val\Drowsy\3935656_dms_drowsy_2.mp4</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>147</v>
+        <v>291</v>
       </c>
       <c r="C5" t="n">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="D5" t="n">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="E5" t="n">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="F5" t="n">
         <v>10</v>
@@ -556,20 +556,20 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>dataset/val\Distraction\3936959_dms_drowsy_1.mp4</t>
+          <t>dataset/val\Drowsy\3937751_dms_drowsy_5.mp4</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>226</v>
+        <v>267</v>
       </c>
       <c r="C6" t="n">
-        <v>142</v>
+        <v>178</v>
       </c>
       <c r="D6" t="n">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="E6" t="n">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>9</v>
@@ -578,20 +578,20 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>dataset/val\Distraction\3955562_dms_drowsy_2.mp4</t>
+          <t>dataset/val\Drowsy\3953799_dms_drowsy_2.mp4</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="C7" t="n">
-        <v>122</v>
+        <v>269</v>
       </c>
       <c r="D7" t="n">
-        <v>177</v>
+        <v>13</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
         <v>9</v>
@@ -600,20 +600,20 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>dataset/val\Distraction\3957456_dms_drowsy_1.mp4</t>
+          <t>dataset/val\Drowsy\3954648_dms_drowsy_23.mp4</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>316</v>
+        <v>291</v>
       </c>
       <c r="C8" t="n">
-        <v>173</v>
+        <v>270</v>
       </c>
       <c r="D8" t="n">
-        <v>143</v>
+        <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>10</v>
@@ -622,17 +622,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>dataset/val\Distraction\3957456_dms_drowsy_2.mp4</t>
+          <t>dataset/val\Drowsy\3958643_dms_drowsy_7.mp4</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>316</v>
+        <v>293</v>
       </c>
       <c r="C9" t="n">
-        <v>173</v>
+        <v>260</v>
       </c>
       <c r="D9" t="n">
-        <v>143</v>
+        <v>33</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -644,264 +644,44 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>dataset/val\Distraction\3958150_dms_drowsy_1.mp4</t>
+          <t>dataset/val\Drowsy\3958754_dms_drowsy_9.mp4</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="C10" t="n">
-        <v>126</v>
+        <v>36</v>
       </c>
       <c r="D10" t="n">
-        <v>186</v>
+        <v>262</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F10" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>dataset/val\Distraction\3958754_dms_drowsy_3.mp4</t>
+          <t>dataset/val\Drowsy\3962857_dms_drowsy_1.mp4</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="C11" t="n">
-        <v>192</v>
+        <v>292</v>
       </c>
       <c r="D11" t="n">
-        <v>111</v>
+        <v>9</v>
       </c>
       <c r="E11" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>dataset/val\Drowsy\360326202501_dms_drowsy_12.mp4</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>231</v>
-      </c>
-      <c r="C12" t="n">
-        <v>197</v>
-      </c>
-      <c r="D12" t="n">
-        <v>32</v>
-      </c>
-      <c r="E12" t="n">
-        <v>2</v>
-      </c>
-      <c r="F12" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>dataset/val\Drowsy\3934336_dms_drowsy_1.mp4</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>306</v>
-      </c>
-      <c r="C13" t="n">
-        <v>299</v>
-      </c>
-      <c r="D13" t="n">
-        <v>6</v>
-      </c>
-      <c r="E13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>dataset/val\Drowsy\3935656_dms_drowsy_1.mp4</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>301</v>
-      </c>
-      <c r="C14" t="n">
-        <v>155</v>
-      </c>
-      <c r="D14" t="n">
-        <v>94</v>
-      </c>
-      <c r="E14" t="n">
-        <v>52</v>
-      </c>
-      <c r="F14" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>dataset/val\Drowsy\3935656_dms_drowsy_2.mp4</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>291</v>
-      </c>
-      <c r="C15" t="n">
-        <v>148</v>
-      </c>
-      <c r="D15" t="n">
-        <v>83</v>
-      </c>
-      <c r="E15" t="n">
-        <v>60</v>
-      </c>
-      <c r="F15" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>dataset/val\Drowsy\3937751_dms_drowsy_5.mp4</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>267</v>
-      </c>
-      <c r="C16" t="n">
-        <v>178</v>
-      </c>
-      <c r="D16" t="n">
-        <v>76</v>
-      </c>
-      <c r="E16" t="n">
-        <v>13</v>
-      </c>
-      <c r="F16" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>dataset/val\Drowsy\3953799_dms_drowsy_2.mp4</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>282</v>
-      </c>
-      <c r="C17" t="n">
-        <v>269</v>
-      </c>
-      <c r="D17" t="n">
-        <v>13</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>dataset/val\Drowsy\3954648_dms_drowsy_23.mp4</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>291</v>
-      </c>
-      <c r="C18" t="n">
-        <v>270</v>
-      </c>
-      <c r="D18" t="n">
-        <v>14</v>
-      </c>
-      <c r="E18" t="n">
-        <v>7</v>
-      </c>
-      <c r="F18" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>dataset/val\Drowsy\3958643_dms_drowsy_7.mp4</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>293</v>
-      </c>
-      <c r="C19" t="n">
-        <v>260</v>
-      </c>
-      <c r="D19" t="n">
-        <v>33</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>dataset/val\Drowsy\3958754_dms_drowsy_9.mp4</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>306</v>
-      </c>
-      <c r="C20" t="n">
-        <v>36</v>
-      </c>
-      <c r="D20" t="n">
-        <v>262</v>
-      </c>
-      <c r="E20" t="n">
-        <v>8</v>
-      </c>
-      <c r="F20" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>dataset/val\Drowsy\3962857_dms_drowsy_1.mp4</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>301</v>
-      </c>
-      <c r="C21" t="n">
-        <v>292</v>
-      </c>
-      <c r="D21" t="n">
-        <v>9</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>